<commit_message>
added images some changes
</commit_message>
<xml_diff>
--- a/storage/app/category_list.xlsx
+++ b/storage/app/category_list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="180">
   <si>
     <t>id</t>
   </si>
@@ -41,178 +41,520 @@
     <t>commission_rate</t>
   </si>
   <si>
-    <t>Women Fashion</t>
-  </si>
-  <si>
-    <t>women-fashion</t>
-  </si>
-  <si>
-    <t>Men Fashion</t>
-  </si>
-  <si>
-    <t>men-fashion</t>
-  </si>
-  <si>
-    <t>Bags</t>
-  </si>
-  <si>
-    <t>bags</t>
-  </si>
-  <si>
-    <t>Watch</t>
-  </si>
-  <si>
-    <t>watch</t>
-  </si>
-  <si>
-    <t>Bikes</t>
-  </si>
-  <si>
-    <t>bikes</t>
-  </si>
-  <si>
-    <t>Shoes</t>
-  </si>
-  <si>
-    <t>shoes</t>
-  </si>
-  <si>
-    <t>Men Shoes</t>
-  </si>
-  <si>
-    <t>men-shoes</t>
-  </si>
-  <si>
-    <t>Women Shoes</t>
-  </si>
-  <si>
-    <t>women-shoes</t>
-  </si>
-  <si>
-    <t>Furnitures</t>
-  </si>
-  <si>
-    <t>furnitures</t>
-  </si>
-  <si>
-    <t>Sofa</t>
-  </si>
-  <si>
-    <t>sofa</t>
-  </si>
-  <si>
-    <t>Automobiles &amp; bikes</t>
-  </si>
-  <si>
-    <t>automobiles-bikes</t>
-  </si>
-  <si>
-    <t>Cars</t>
-  </si>
-  <si>
-    <t>cars</t>
-  </si>
-  <si>
-    <t>Sun Glasses</t>
-  </si>
-  <si>
-    <t>sun-glasses</t>
-  </si>
-  <si>
-    <t>Helmet</t>
-  </si>
-  <si>
-    <t>helmet</t>
-  </si>
-  <si>
-    <t>Computer</t>
-  </si>
-  <si>
-    <t>computer</t>
-  </si>
-  <si>
-    <t>Monitor</t>
-  </si>
-  <si>
-    <t>monitor</t>
-  </si>
-  <si>
-    <t>Laptop</t>
-  </si>
-  <si>
-    <t>laptop</t>
-  </si>
-  <si>
-    <t>SSD</t>
-  </si>
-  <si>
-    <t>ssd</t>
-  </si>
-  <si>
-    <t>Mobiles</t>
-  </si>
-  <si>
-    <t>mobiles</t>
-  </si>
-  <si>
-    <t>Camera</t>
-  </si>
-  <si>
-    <t>camera</t>
-  </si>
-  <si>
-    <t>Ip Camera</t>
-  </si>
-  <si>
-    <t>ip-camera</t>
-  </si>
-  <si>
-    <t>Toys &amp; Hobbies</t>
-  </si>
-  <si>
-    <t>toyshobbies</t>
-  </si>
-  <si>
-    <t>Shari</t>
-  </si>
-  <si>
-    <t>shari</t>
-  </si>
-  <si>
-    <t>BiCycle</t>
-  </si>
-  <si>
-    <t>bicycle</t>
-  </si>
-  <si>
-    <t>Wooden Furniture</t>
-  </si>
-  <si>
-    <t>wooden-furniture</t>
-  </si>
-  <si>
-    <t>Software</t>
-  </si>
-  <si>
-    <t>software</t>
-  </si>
-  <si>
-    <t>Electronics</t>
-  </si>
-  <si>
-    <t>electronics</t>
-  </si>
-  <si>
-    <t>Tablet Device</t>
-  </si>
-  <si>
-    <t>tablet-device</t>
-  </si>
-  <si>
-    <t>{"en":"T-Shirt"}</t>
-  </si>
-  <si>
-    <t>t-shirt</t>
+    <t>Home &amp; Living</t>
+  </si>
+  <si>
+    <t>home-&amp;-living</t>
+  </si>
+  <si>
+    <t>Home Decors</t>
+  </si>
+  <si>
+    <t>home-decors</t>
+  </si>
+  <si>
+    <t>Kitchen &amp; Dining</t>
+  </si>
+  <si>
+    <t>kitchen-&amp;-dining</t>
+  </si>
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
+    <t>accessories</t>
+  </si>
+  <si>
+    <t>Pooja Essentials</t>
+  </si>
+  <si>
+    <t>pooja-essentials</t>
+  </si>
+  <si>
+    <t>Furnishings</t>
+  </si>
+  <si>
+    <t>-furnishings</t>
+  </si>
+  <si>
+    <t>Home Essentials</t>
+  </si>
+  <si>
+    <t>home-essentials</t>
+  </si>
+  <si>
+    <t>Festive Decor</t>
+  </si>
+  <si>
+    <t>festive-decor</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>women</t>
+  </si>
+  <si>
+    <t>Jewellery</t>
+  </si>
+  <si>
+    <t>jewellery</t>
+  </si>
+  <si>
+    <t>Footware</t>
+  </si>
+  <si>
+    <t>footware</t>
+  </si>
+  <si>
+    <t>Sarees</t>
+  </si>
+  <si>
+    <t>sarees</t>
+  </si>
+  <si>
+    <t>Bags &amp; Pouches</t>
+  </si>
+  <si>
+    <t>bags-&amp;-pouches</t>
+  </si>
+  <si>
+    <t>Personal Care</t>
+  </si>
+  <si>
+    <t>personal-care</t>
+  </si>
+  <si>
+    <t>Toys</t>
+  </si>
+  <si>
+    <t>toys</t>
+  </si>
+  <si>
+    <t>Channapatna Toys</t>
+  </si>
+  <si>
+    <t>channapatna-toys</t>
+  </si>
+  <si>
+    <t>Soft Toys</t>
+  </si>
+  <si>
+    <t>soft-toys</t>
+  </si>
+  <si>
+    <t>Paintings</t>
+  </si>
+  <si>
+    <t>paintings</t>
+  </si>
+  <si>
+    <t>Wooden Paintings</t>
+  </si>
+  <si>
+    <t>wooden-paintings</t>
+  </si>
+  <si>
+    <t>Framed Paintings</t>
+  </si>
+  <si>
+    <t>framed-paintings</t>
+  </si>
+  <si>
+    <t>Idols &amp; Figurines</t>
+  </si>
+  <si>
+    <t>idols-&amp;-figurines</t>
+  </si>
+  <si>
+    <t>Wall Decor</t>
+  </si>
+  <si>
+    <t>wall-decor</t>
+  </si>
+  <si>
+    <t>Handcreaft Items</t>
+  </si>
+  <si>
+    <t>handcreaft-items</t>
+  </si>
+  <si>
+    <t>Lamps &amp; Lightning</t>
+  </si>
+  <si>
+    <t>lamps-&amp;-lightning</t>
+  </si>
+  <si>
+    <t>Home Accents</t>
+  </si>
+  <si>
+    <t>home-accents</t>
+  </si>
+  <si>
+    <t>Wooden Artwork</t>
+  </si>
+  <si>
+    <t>wooden-artwork</t>
+  </si>
+  <si>
+    <t>Drinkware</t>
+  </si>
+  <si>
+    <t>drinkware</t>
+  </si>
+  <si>
+    <t>Tableware</t>
+  </si>
+  <si>
+    <t>tableware</t>
+  </si>
+  <si>
+    <t>Cutlery</t>
+  </si>
+  <si>
+    <t>cutlery</t>
+  </si>
+  <si>
+    <t>Kitchen Storage</t>
+  </si>
+  <si>
+    <t>kitchen-storage</t>
+  </si>
+  <si>
+    <t>Beauty and Personal Care</t>
+  </si>
+  <si>
+    <t>beauty-and-personal-care</t>
+  </si>
+  <si>
+    <t>Wired Fiber Basket</t>
+  </si>
+  <si>
+    <t>wired-fiber-basket</t>
+  </si>
+  <si>
+    <t>Bamboo Brooms</t>
+  </si>
+  <si>
+    <t>bamboo-brooms</t>
+  </si>
+  <si>
+    <t>Mats</t>
+  </si>
+  <si>
+    <t>mats</t>
+  </si>
+  <si>
+    <t>Bags Collection</t>
+  </si>
+  <si>
+    <t>bags-collection</t>
+  </si>
+  <si>
+    <t>Bridal Headband</t>
+  </si>
+  <si>
+    <t>bridal-headband</t>
+  </si>
+  <si>
+    <t>Hair Accesories</t>
+  </si>
+  <si>
+    <t>hair-accesories</t>
+  </si>
+  <si>
+    <t>Penstand</t>
+  </si>
+  <si>
+    <t>penstand</t>
+  </si>
+  <si>
+    <t>Keychains</t>
+  </si>
+  <si>
+    <t>keychains</t>
+  </si>
+  <si>
+    <t>Pooja Thali Set</t>
+  </si>
+  <si>
+    <t>pooja-thali-set</t>
+  </si>
+  <si>
+    <t>God Idols</t>
+  </si>
+  <si>
+    <t>god-idols</t>
+  </si>
+  <si>
+    <t>Designer Diyas</t>
+  </si>
+  <si>
+    <t>designer-diyas</t>
+  </si>
+  <si>
+    <t>Garlands</t>
+  </si>
+  <si>
+    <t>garlands</t>
+  </si>
+  <si>
+    <t>Gold Idols</t>
+  </si>
+  <si>
+    <t>gold-idols</t>
+  </si>
+  <si>
+    <t>Pooja Thali</t>
+  </si>
+  <si>
+    <t>pooja-thali</t>
+  </si>
+  <si>
+    <t>Incense Sticks</t>
+  </si>
+  <si>
+    <t>incense-sticks</t>
+  </si>
+  <si>
+    <t>Cushion Cover</t>
+  </si>
+  <si>
+    <t>cushion-cover</t>
+  </si>
+  <si>
+    <t>Necklace</t>
+  </si>
+  <si>
+    <t>necklace</t>
+  </si>
+  <si>
+    <t>Bangles</t>
+  </si>
+  <si>
+    <t>bangles</t>
+  </si>
+  <si>
+    <t>Handbands</t>
+  </si>
+  <si>
+    <t>handbands</t>
+  </si>
+  <si>
+    <t>Earrings</t>
+  </si>
+  <si>
+    <t>earrings</t>
+  </si>
+  <si>
+    <t>Kolhapuri Chappal</t>
+  </si>
+  <si>
+    <t>kolhapuri-chappal</t>
+  </si>
+  <si>
+    <t>Udupi</t>
+  </si>
+  <si>
+    <t>-udupi</t>
+  </si>
+  <si>
+    <t>Chanderi</t>
+  </si>
+  <si>
+    <t>chanderi</t>
+  </si>
+  <si>
+    <t>Cotton Silk</t>
+  </si>
+  <si>
+    <t>cotton-silk</t>
+  </si>
+  <si>
+    <t>Ilkal</t>
+  </si>
+  <si>
+    <t>ilkal</t>
+  </si>
+  <si>
+    <t>Handbag</t>
+  </si>
+  <si>
+    <t>handbag</t>
+  </si>
+  <si>
+    <t>Slingbag</t>
+  </si>
+  <si>
+    <t>slingbag</t>
+  </si>
+  <si>
+    <t>Handpurse</t>
+  </si>
+  <si>
+    <t>handpurse</t>
+  </si>
+  <si>
+    <t>Ladies Pouch</t>
+  </si>
+  <si>
+    <t>ladies-pouch</t>
+  </si>
+  <si>
+    <t>Beauty Products</t>
+  </si>
+  <si>
+    <t>beauty-products</t>
+  </si>
+  <si>
+    <t>Herbal Soap</t>
+  </si>
+  <si>
+    <t>herbal-soap</t>
+  </si>
+  <si>
+    <t>Sanitary Pads</t>
+  </si>
+  <si>
+    <t>sanitary-pads</t>
+  </si>
+  <si>
+    <t>Kids</t>
+  </si>
+  <si>
+    <t>kids</t>
+  </si>
+  <si>
+    <t>Baby Beds</t>
+  </si>
+  <si>
+    <t>baby-beds</t>
+  </si>
+  <si>
+    <t>Unisex</t>
+  </si>
+  <si>
+    <t>unisex</t>
+  </si>
+  <si>
+    <t>Mysore Peta</t>
+  </si>
+  <si>
+    <t>mysore-peta</t>
+  </si>
+  <si>
+    <t>Shawls</t>
+  </si>
+  <si>
+    <t>shawls</t>
+  </si>
+  <si>
+    <t>Lambani Bags</t>
+  </si>
+  <si>
+    <t>lambani-bags</t>
+  </si>
+  <si>
+    <t>Lambani Apparels</t>
+  </si>
+  <si>
+    <t>lambani-apparels</t>
+  </si>
+  <si>
+    <t>Lambani Dress</t>
+  </si>
+  <si>
+    <t>lambani-dress</t>
+  </si>
+  <si>
+    <t>Lambani Purse</t>
+  </si>
+  <si>
+    <t>lambani-purse</t>
+  </si>
+  <si>
+    <t>Pickles</t>
+  </si>
+  <si>
+    <t>pickles</t>
+  </si>
+  <si>
+    <t>Condiments</t>
+  </si>
+  <si>
+    <t>condiments</t>
+  </si>
+  <si>
+    <t>Beverages</t>
+  </si>
+  <si>
+    <t>beverages</t>
+  </si>
+  <si>
+    <t>Non-Alcoholic Drinks</t>
+  </si>
+  <si>
+    <t>non-alcoholic-drinks</t>
+  </si>
+  <si>
+    <t>Essential</t>
+  </si>
+  <si>
+    <t>essential</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>oil</t>
+  </si>
+  <si>
+    <t>Ghee</t>
+  </si>
+  <si>
+    <t>ghee</t>
+  </si>
+  <si>
+    <t>Papad</t>
+  </si>
+  <si>
+    <t>papad</t>
+  </si>
+  <si>
+    <t>Processed &amp; Packed foods</t>
+  </si>
+  <si>
+    <t>processed-&amp;-packed-foods</t>
+  </si>
+  <si>
+    <t>Spices</t>
+  </si>
+  <si>
+    <t>spices</t>
+  </si>
+  <si>
+    <t>Roti and Chutney</t>
+  </si>
+  <si>
+    <t>roti-and-chutney</t>
+  </si>
+  <si>
+    <t>Sweets</t>
+  </si>
+  <si>
+    <t>sweets</t>
+  </si>
+  <si>
+    <t>Tea &amp; Coffee</t>
+  </si>
+  <si>
+    <t>tea-&amp;-coffee</t>
+  </si>
+  <si>
+    <t>Apparels</t>
+  </si>
+  <si>
+    <t>apparels</t>
   </si>
 </sst>
 </file>
@@ -240,15 +582,19 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,7 +894,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -584,7 +930,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -595,13 +941,16 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="G2">
+        <v>0.0</v>
+      </c>
       <c r="H2">
-        <v>5</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -609,11 +958,17 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>0.0</v>
       </c>
       <c r="H3">
-        <v>5</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -626,11 +981,17 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0.0</v>
       </c>
       <c r="H4">
-        <v>5</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -643,14 +1004,17 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>0.0</v>
       </c>
       <c r="H5">
-        <v>6</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -664,13 +1028,16 @@
         <v>17</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
+      <c r="G6">
+        <v>0.0</v>
+      </c>
       <c r="H6">
-        <v>2</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -683,11 +1050,17 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>0.0</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -701,16 +1074,16 @@
         <v>21</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
-      <c r="F8">
-        <v>2</v>
+      <c r="G8">
+        <v>0.0</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -724,13 +1097,16 @@
         <v>23</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
+      <c r="G9">
+        <v>0.0</v>
+      </c>
       <c r="H9">
-        <v>5</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -746,8 +1122,11 @@
       <c r="E10">
         <v>1</v>
       </c>
+      <c r="G10">
+        <v>0.0</v>
+      </c>
       <c r="H10">
-        <v>5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -766,11 +1145,11 @@
       <c r="E11">
         <v>2</v>
       </c>
-      <c r="F11">
-        <v>2</v>
+      <c r="G11">
+        <v>0.0</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -783,11 +1162,17 @@
       <c r="C12" t="s">
         <v>29</v>
       </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
       <c r="E12">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>0.0</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -801,13 +1186,16 @@
         <v>31</v>
       </c>
       <c r="D13">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E13">
         <v>2</v>
       </c>
+      <c r="G13">
+        <v>0.0</v>
+      </c>
       <c r="H13">
-        <v>3</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -820,11 +1208,17 @@
       <c r="C14" t="s">
         <v>33</v>
       </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
       <c r="E14">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>0.0</v>
       </c>
       <c r="H14">
-        <v>5</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -838,16 +1232,16 @@
         <v>35</v>
       </c>
       <c r="D15">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
-      <c r="F15">
-        <v>1</v>
+      <c r="G15">
+        <v>0.0</v>
       </c>
       <c r="H15">
-        <v>5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -863,6 +1257,12 @@
       <c r="E16">
         <v>1</v>
       </c>
+      <c r="G16">
+        <v>0.0</v>
+      </c>
+      <c r="H16">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
@@ -875,10 +1275,16 @@
         <v>39</v>
       </c>
       <c r="D17">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E17">
         <v>2</v>
+      </c>
+      <c r="G17">
+        <v>0.0</v>
+      </c>
+      <c r="H17">
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -892,10 +1298,16 @@
         <v>41</v>
       </c>
       <c r="D18">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E18">
         <v>2</v>
+      </c>
+      <c r="G18">
+        <v>0.0</v>
+      </c>
+      <c r="H18">
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -911,8 +1323,11 @@
       <c r="E19">
         <v>1</v>
       </c>
+      <c r="G19">
+        <v>0.0</v>
+      </c>
       <c r="H19">
-        <v>1</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -926,10 +1341,16 @@
         <v>45</v>
       </c>
       <c r="D20">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E20">
         <v>2</v>
+      </c>
+      <c r="G20">
+        <v>0.0</v>
+      </c>
+      <c r="H20">
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -942,8 +1363,17 @@
       <c r="C21" t="s">
         <v>47</v>
       </c>
+      <c r="D21">
+        <v>18</v>
+      </c>
       <c r="E21">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>0.0</v>
+      </c>
+      <c r="H21">
+        <v>5.0</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -957,13 +1387,16 @@
         <v>49</v>
       </c>
       <c r="D22">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>0.0</v>
       </c>
       <c r="H22">
-        <v>3</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -976,16 +1409,22 @@
       <c r="C23" t="s">
         <v>51</v>
       </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
       <c r="E23">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>0.0</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>52</v>
@@ -997,12 +1436,18 @@
         <v>1</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>0.0</v>
+      </c>
+      <c r="H24">
+        <v>0.0</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>54</v>
@@ -1010,13 +1455,22 @@
       <c r="C25" t="s">
         <v>55</v>
       </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
       <c r="E25">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>0.0</v>
+      </c>
+      <c r="H25">
+        <v>0.0</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>56</v>
@@ -1025,15 +1479,21 @@
         <v>57</v>
       </c>
       <c r="D26">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>0.0</v>
+      </c>
+      <c r="H26">
+        <v>0.0</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>58</v>
@@ -1041,13 +1501,22 @@
       <c r="C27" t="s">
         <v>59</v>
       </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
       <c r="E27">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>0.0</v>
+      </c>
+      <c r="H27">
+        <v>0.0</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>60</v>
@@ -1055,13 +1524,22 @@
       <c r="C28" t="s">
         <v>61</v>
       </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
       <c r="E28">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>0.0</v>
+      </c>
+      <c r="H28">
+        <v>0.0</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>62</v>
@@ -1070,15 +1548,21 @@
         <v>63</v>
       </c>
       <c r="D29">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>0.0</v>
+      </c>
+      <c r="H29">
+        <v>0.0</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>64</v>
@@ -1086,12 +1570,1307 @@
       <c r="C30" t="s">
         <v>65</v>
       </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
       <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <v>0.0</v>
+      </c>
+      <c r="H30">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <v>0.0</v>
+      </c>
+      <c r="H31">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>0.0</v>
+      </c>
+      <c r="H32">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33">
+        <v>7</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="G33">
+        <v>0.0</v>
+      </c>
+      <c r="H33">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34">
+        <v>7</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="G34">
+        <v>0.0</v>
+      </c>
+      <c r="H34">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35">
+        <v>7</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="G35">
+        <v>0.0</v>
+      </c>
+      <c r="H35">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <v>0.0</v>
+      </c>
+      <c r="H36">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <v>0.0</v>
+      </c>
+      <c r="H37">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="G38">
+        <v>0.0</v>
+      </c>
+      <c r="H38">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="G39">
+        <v>0.0</v>
+      </c>
+      <c r="H39">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>0.0</v>
+      </c>
+      <c r="H40">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="G41">
+        <v>0.0</v>
+      </c>
+      <c r="H41">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="G42">
+        <v>0.0</v>
+      </c>
+      <c r="H42">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="G43">
+        <v>0.0</v>
+      </c>
+      <c r="H43">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44">
+        <v>8</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="G44">
+        <v>0.0</v>
+      </c>
+      <c r="H44">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="G45">
+        <v>0.0</v>
+      </c>
+      <c r="H45">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="G46">
+        <v>0.0</v>
+      </c>
+      <c r="H46">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="G47">
+        <v>0.0</v>
+      </c>
+      <c r="H47">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48">
+        <v>6</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+      <c r="G48">
+        <v>0.0</v>
+      </c>
+      <c r="H48">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49">
+        <v>10</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="G49">
+        <v>0.0</v>
+      </c>
+      <c r="H49">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50">
+        <v>10</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="G50">
+        <v>0.0</v>
+      </c>
+      <c r="H50">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51">
+        <v>10</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <v>0.0</v>
+      </c>
+      <c r="H51">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52">
+        <v>10</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+      <c r="G52">
+        <v>0.0</v>
+      </c>
+      <c r="H52">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" t="s">
+        <v>111</v>
+      </c>
+      <c r="D53">
+        <v>11</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="G53">
+        <v>0.0</v>
+      </c>
+      <c r="H53">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54">
+        <v>12</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="G54">
+        <v>0.0</v>
+      </c>
+      <c r="H54">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" t="s">
+        <v>115</v>
+      </c>
+      <c r="D55">
+        <v>12</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <v>0.0</v>
+      </c>
+      <c r="H55">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>116</v>
+      </c>
+      <c r="C56" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56">
+        <v>12</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="G56">
+        <v>0.0</v>
+      </c>
+      <c r="H56">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57">
+        <v>12</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <v>0.0</v>
+      </c>
+      <c r="H57">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" t="s">
+        <v>121</v>
+      </c>
+      <c r="D58">
+        <v>13</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="G58">
+        <v>0.0</v>
+      </c>
+      <c r="H58">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59">
+        <v>13</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+      <c r="G59">
+        <v>0.0</v>
+      </c>
+      <c r="H59">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>124</v>
+      </c>
+      <c r="C60" t="s">
+        <v>125</v>
+      </c>
+      <c r="D60">
+        <v>13</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+      <c r="G60">
+        <v>0.0</v>
+      </c>
+      <c r="H60">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" t="s">
+        <v>127</v>
+      </c>
+      <c r="D61">
+        <v>13</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+      <c r="G61">
+        <v>0.0</v>
+      </c>
+      <c r="H61">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62">
+        <v>14</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="G62">
+        <v>0.0</v>
+      </c>
+      <c r="H62">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>130</v>
+      </c>
+      <c r="C63" t="s">
+        <v>131</v>
+      </c>
+      <c r="D63">
+        <v>14</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="G63">
+        <v>0.0</v>
+      </c>
+      <c r="H63">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" t="s">
+        <v>133</v>
+      </c>
+      <c r="D64">
+        <v>14</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="G64">
+        <v>0.0</v>
+      </c>
+      <c r="H64">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>134</v>
+      </c>
+      <c r="C65" t="s">
+        <v>135</v>
+      </c>
+      <c r="E65">
         <v>1</v>
       </c>
+      <c r="G65">
+        <v>0.0</v>
+      </c>
+      <c r="H65">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>136</v>
+      </c>
+      <c r="C66" t="s">
+        <v>137</v>
+      </c>
+      <c r="D66">
+        <v>65</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="G66">
+        <v>0.0</v>
+      </c>
+      <c r="H66">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" t="s">
+        <v>139</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>0.0</v>
+      </c>
+      <c r="H67">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>140</v>
+      </c>
+      <c r="C68" t="s">
+        <v>141</v>
+      </c>
+      <c r="D68">
+        <v>67</v>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="G68">
+        <v>0.0</v>
+      </c>
+      <c r="H68">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="B69" t="s">
+        <v>142</v>
+      </c>
+      <c r="C69" t="s">
+        <v>143</v>
+      </c>
+      <c r="D69">
+        <v>67</v>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+      <c r="G69">
+        <v>0.0</v>
+      </c>
+      <c r="H69">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70">
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
+        <v>144</v>
+      </c>
+      <c r="C70" t="s">
+        <v>145</v>
+      </c>
+      <c r="D70">
+        <v>67</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="G70">
+        <v>0.0</v>
+      </c>
+      <c r="H70">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71">
+        <v>72</v>
+      </c>
+      <c r="B71" t="s">
+        <v>146</v>
+      </c>
+      <c r="C71" t="s">
+        <v>147</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>0.0</v>
+      </c>
+      <c r="H71">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>148</v>
+      </c>
+      <c r="C72" t="s">
+        <v>149</v>
+      </c>
+      <c r="D72">
+        <v>72</v>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+      <c r="G72">
+        <v>0.0</v>
+      </c>
+      <c r="H72">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73">
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
+        <v>150</v>
+      </c>
+      <c r="C73" t="s">
+        <v>151</v>
+      </c>
+      <c r="D73">
+        <v>72</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+      <c r="G73">
+        <v>0.0</v>
+      </c>
+      <c r="H73">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74">
+        <v>75</v>
+      </c>
+      <c r="B74" t="s">
+        <v>152</v>
+      </c>
+      <c r="C74" t="s">
+        <v>153</v>
+      </c>
+      <c r="D74">
+        <v>74</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+      <c r="G74">
+        <v>0.0</v>
+      </c>
+      <c r="H74">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>154</v>
+      </c>
+      <c r="C75" t="s">
+        <v>155</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>0.0</v>
+      </c>
+      <c r="H75">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>156</v>
+      </c>
+      <c r="C76" t="s">
+        <v>157</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="G76">
+        <v>0.0</v>
+      </c>
+      <c r="H76">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77">
+        <v>77</v>
+      </c>
+      <c r="B77" t="s">
+        <v>158</v>
+      </c>
+      <c r="C77" t="s">
+        <v>159</v>
+      </c>
+      <c r="D77">
+        <v>76</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="G77">
+        <v>0.0</v>
+      </c>
+      <c r="H77">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>160</v>
+      </c>
+      <c r="C78" t="s">
+        <v>161</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="G78">
+        <v>0.0</v>
+      </c>
+      <c r="H78">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>162</v>
+      </c>
+      <c r="C79" t="s">
+        <v>163</v>
+      </c>
+      <c r="D79">
+        <v>78</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+      <c r="G79">
+        <v>0.0</v>
+      </c>
+      <c r="H79">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>164</v>
+      </c>
+      <c r="C80" t="s">
+        <v>165</v>
+      </c>
+      <c r="D80">
+        <v>78</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="G80">
+        <v>0.0</v>
+      </c>
+      <c r="H80">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>166</v>
+      </c>
+      <c r="C81" t="s">
+        <v>167</v>
+      </c>
+      <c r="D81">
+        <v>78</v>
+      </c>
+      <c r="E81">
+        <v>2</v>
+      </c>
+      <c r="G81">
+        <v>0.0</v>
+      </c>
+      <c r="H81">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>168</v>
+      </c>
+      <c r="C82" t="s">
+        <v>169</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>0.0</v>
+      </c>
+      <c r="H82">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83">
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
+        <v>170</v>
+      </c>
+      <c r="C83" t="s">
+        <v>171</v>
+      </c>
+      <c r="D83">
+        <v>82</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="G83">
+        <v>0.0</v>
+      </c>
+      <c r="H83">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>172</v>
+      </c>
+      <c r="C84" t="s">
+        <v>173</v>
+      </c>
+      <c r="D84">
+        <v>82</v>
+      </c>
+      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="G84">
+        <v>0.0</v>
+      </c>
+      <c r="H84">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>174</v>
+      </c>
+      <c r="C85" t="s">
+        <v>175</v>
+      </c>
+      <c r="D85">
+        <v>82</v>
+      </c>
+      <c r="E85">
+        <v>2</v>
+      </c>
+      <c r="G85">
+        <v>0.0</v>
+      </c>
+      <c r="H85">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" t="s">
+        <v>177</v>
+      </c>
+      <c r="D86">
+        <v>82</v>
+      </c>
+      <c r="E86">
+        <v>2</v>
+      </c>
+      <c r="G86">
+        <v>0.0</v>
+      </c>
+      <c r="H86">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87">
+        <v>64</v>
+      </c>
+      <c r="B87" t="s">
+        <v>178</v>
+      </c>
+      <c r="C87" t="s">
+        <v>179</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="G87">
+        <v>0.0</v>
+      </c>
+      <c r="H87">
+        <v>0.0</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
@@ -1103,5 +2882,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
footer_setting our legal title updating is working at (2024-08-29)
</commit_message>
<xml_diff>
--- a/storage/app/category_list.xlsx
+++ b/storage/app/category_list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="180">
   <si>
     <t>id</t>
   </si>
@@ -41,178 +41,520 @@
     <t>commission_rate</t>
   </si>
   <si>
-    <t>Women Fashion</t>
-  </si>
-  <si>
-    <t>women-fashion</t>
-  </si>
-  <si>
-    <t>Men Fashion</t>
-  </si>
-  <si>
-    <t>men-fashion</t>
-  </si>
-  <si>
-    <t>Bags</t>
-  </si>
-  <si>
-    <t>bags</t>
-  </si>
-  <si>
-    <t>Watch</t>
-  </si>
-  <si>
-    <t>watch</t>
-  </si>
-  <si>
-    <t>Bikes</t>
-  </si>
-  <si>
-    <t>bikes</t>
-  </si>
-  <si>
-    <t>Shoes</t>
-  </si>
-  <si>
-    <t>shoes</t>
-  </si>
-  <si>
-    <t>Men Shoes</t>
-  </si>
-  <si>
-    <t>men-shoes</t>
-  </si>
-  <si>
-    <t>Women Shoes</t>
-  </si>
-  <si>
-    <t>women-shoes</t>
-  </si>
-  <si>
-    <t>Furnitures</t>
-  </si>
-  <si>
-    <t>furnitures</t>
-  </si>
-  <si>
-    <t>Sofa</t>
-  </si>
-  <si>
-    <t>sofa</t>
-  </si>
-  <si>
-    <t>Automobiles &amp; bikes</t>
-  </si>
-  <si>
-    <t>automobiles-bikes</t>
-  </si>
-  <si>
-    <t>Cars</t>
-  </si>
-  <si>
-    <t>cars</t>
-  </si>
-  <si>
-    <t>Sun Glasses</t>
-  </si>
-  <si>
-    <t>sun-glasses</t>
-  </si>
-  <si>
-    <t>Helmet</t>
-  </si>
-  <si>
-    <t>helmet</t>
-  </si>
-  <si>
-    <t>Computer</t>
-  </si>
-  <si>
-    <t>computer</t>
-  </si>
-  <si>
-    <t>Monitor</t>
-  </si>
-  <si>
-    <t>monitor</t>
-  </si>
-  <si>
-    <t>Laptop</t>
-  </si>
-  <si>
-    <t>laptop</t>
-  </si>
-  <si>
-    <t>SSD</t>
-  </si>
-  <si>
-    <t>ssd</t>
-  </si>
-  <si>
-    <t>Mobiles</t>
-  </si>
-  <si>
-    <t>mobiles</t>
-  </si>
-  <si>
-    <t>Camera</t>
-  </si>
-  <si>
-    <t>camera</t>
-  </si>
-  <si>
-    <t>Ip Camera</t>
-  </si>
-  <si>
-    <t>ip-camera</t>
-  </si>
-  <si>
-    <t>Toys &amp; Hobbies</t>
-  </si>
-  <si>
-    <t>toyshobbies</t>
-  </si>
-  <si>
-    <t>Shari</t>
-  </si>
-  <si>
-    <t>shari</t>
-  </si>
-  <si>
-    <t>BiCycle</t>
-  </si>
-  <si>
-    <t>bicycle</t>
-  </si>
-  <si>
-    <t>Wooden Furniture</t>
-  </si>
-  <si>
-    <t>wooden-furniture</t>
-  </si>
-  <si>
-    <t>Software</t>
-  </si>
-  <si>
-    <t>software</t>
-  </si>
-  <si>
-    <t>Electronics</t>
-  </si>
-  <si>
-    <t>electronics</t>
-  </si>
-  <si>
-    <t>Tablet Device</t>
-  </si>
-  <si>
-    <t>tablet-device</t>
-  </si>
-  <si>
-    <t>{"en":"T-Shirt"}</t>
-  </si>
-  <si>
-    <t>t-shirt</t>
+    <t>Home &amp; Living</t>
+  </si>
+  <si>
+    <t>home-&amp;-living</t>
+  </si>
+  <si>
+    <t>Home Decors</t>
+  </si>
+  <si>
+    <t>home-decors</t>
+  </si>
+  <si>
+    <t>Kitchen &amp; Dining</t>
+  </si>
+  <si>
+    <t>kitchen-&amp;-dining</t>
+  </si>
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
+    <t>accessories</t>
+  </si>
+  <si>
+    <t>Pooja Essentials</t>
+  </si>
+  <si>
+    <t>pooja-essentials</t>
+  </si>
+  <si>
+    <t>Furnishings</t>
+  </si>
+  <si>
+    <t>-furnishings</t>
+  </si>
+  <si>
+    <t>Home Essentials</t>
+  </si>
+  <si>
+    <t>home-essentials</t>
+  </si>
+  <si>
+    <t>Festive Decor</t>
+  </si>
+  <si>
+    <t>festive-decor</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>women</t>
+  </si>
+  <si>
+    <t>Jewellery</t>
+  </si>
+  <si>
+    <t>jewellery</t>
+  </si>
+  <si>
+    <t>Footware</t>
+  </si>
+  <si>
+    <t>footware</t>
+  </si>
+  <si>
+    <t>Sarees</t>
+  </si>
+  <si>
+    <t>sarees</t>
+  </si>
+  <si>
+    <t>Bags &amp; Pouches</t>
+  </si>
+  <si>
+    <t>bags-&amp;-pouches</t>
+  </si>
+  <si>
+    <t>Personal Care</t>
+  </si>
+  <si>
+    <t>personal-care</t>
+  </si>
+  <si>
+    <t>Toys</t>
+  </si>
+  <si>
+    <t>toys</t>
+  </si>
+  <si>
+    <t>Channapatna Toys</t>
+  </si>
+  <si>
+    <t>channapatna-toys</t>
+  </si>
+  <si>
+    <t>Soft Toys</t>
+  </si>
+  <si>
+    <t>soft-toys</t>
+  </si>
+  <si>
+    <t>Paintings</t>
+  </si>
+  <si>
+    <t>paintings</t>
+  </si>
+  <si>
+    <t>Wooden Paintings</t>
+  </si>
+  <si>
+    <t>wooden-paintings</t>
+  </si>
+  <si>
+    <t>Framed Paintings</t>
+  </si>
+  <si>
+    <t>framed-paintings</t>
+  </si>
+  <si>
+    <t>Idols &amp; Figurines</t>
+  </si>
+  <si>
+    <t>idols-&amp;-figurines</t>
+  </si>
+  <si>
+    <t>Wall Decor</t>
+  </si>
+  <si>
+    <t>wall-decor</t>
+  </si>
+  <si>
+    <t>Handcreaft Items</t>
+  </si>
+  <si>
+    <t>handcreaft-items</t>
+  </si>
+  <si>
+    <t>Lamps &amp; Lightning</t>
+  </si>
+  <si>
+    <t>lamps-&amp;-lightning</t>
+  </si>
+  <si>
+    <t>Home Accents</t>
+  </si>
+  <si>
+    <t>home-accents</t>
+  </si>
+  <si>
+    <t>Wooden Artwork</t>
+  </si>
+  <si>
+    <t>wooden-artwork</t>
+  </si>
+  <si>
+    <t>Drinkware</t>
+  </si>
+  <si>
+    <t>drinkware</t>
+  </si>
+  <si>
+    <t>Tableware</t>
+  </si>
+  <si>
+    <t>tableware</t>
+  </si>
+  <si>
+    <t>Cutlery</t>
+  </si>
+  <si>
+    <t>cutlery</t>
+  </si>
+  <si>
+    <t>Kitchen Storage</t>
+  </si>
+  <si>
+    <t>kitchen-storage</t>
+  </si>
+  <si>
+    <t>Beauty and Personal Care</t>
+  </si>
+  <si>
+    <t>beauty-and-personal-care</t>
+  </si>
+  <si>
+    <t>Wired Fiber Basket</t>
+  </si>
+  <si>
+    <t>wired-fiber-basket</t>
+  </si>
+  <si>
+    <t>Bamboo Brooms</t>
+  </si>
+  <si>
+    <t>bamboo-brooms</t>
+  </si>
+  <si>
+    <t>Mats</t>
+  </si>
+  <si>
+    <t>mats</t>
+  </si>
+  <si>
+    <t>Bags Collection</t>
+  </si>
+  <si>
+    <t>bags-collection</t>
+  </si>
+  <si>
+    <t>Bridal Headband</t>
+  </si>
+  <si>
+    <t>bridal-headband</t>
+  </si>
+  <si>
+    <t>Hair Accesories</t>
+  </si>
+  <si>
+    <t>hair-accesories</t>
+  </si>
+  <si>
+    <t>Penstand</t>
+  </si>
+  <si>
+    <t>penstand</t>
+  </si>
+  <si>
+    <t>Keychains</t>
+  </si>
+  <si>
+    <t>keychains</t>
+  </si>
+  <si>
+    <t>Pooja Thali Set</t>
+  </si>
+  <si>
+    <t>pooja-thali-set</t>
+  </si>
+  <si>
+    <t>God Idols</t>
+  </si>
+  <si>
+    <t>god-idols</t>
+  </si>
+  <si>
+    <t>Designer Diyas</t>
+  </si>
+  <si>
+    <t>designer-diyas</t>
+  </si>
+  <si>
+    <t>Garlands</t>
+  </si>
+  <si>
+    <t>garlands</t>
+  </si>
+  <si>
+    <t>Gold Idols</t>
+  </si>
+  <si>
+    <t>gold-idols</t>
+  </si>
+  <si>
+    <t>Pooja Thali</t>
+  </si>
+  <si>
+    <t>pooja-thali</t>
+  </si>
+  <si>
+    <t>Incense Sticks</t>
+  </si>
+  <si>
+    <t>incense-sticks</t>
+  </si>
+  <si>
+    <t>Cushion Cover</t>
+  </si>
+  <si>
+    <t>cushion-cover</t>
+  </si>
+  <si>
+    <t>Necklace</t>
+  </si>
+  <si>
+    <t>necklace</t>
+  </si>
+  <si>
+    <t>Bangles</t>
+  </si>
+  <si>
+    <t>bangles</t>
+  </si>
+  <si>
+    <t>Handbands</t>
+  </si>
+  <si>
+    <t>handbands</t>
+  </si>
+  <si>
+    <t>Earrings</t>
+  </si>
+  <si>
+    <t>earrings</t>
+  </si>
+  <si>
+    <t>Kolhapuri Chappal</t>
+  </si>
+  <si>
+    <t>kolhapuri-chappal</t>
+  </si>
+  <si>
+    <t>Udupi</t>
+  </si>
+  <si>
+    <t>-udupi</t>
+  </si>
+  <si>
+    <t>Chanderi</t>
+  </si>
+  <si>
+    <t>chanderi</t>
+  </si>
+  <si>
+    <t>Cotton Silk</t>
+  </si>
+  <si>
+    <t>cotton-silk</t>
+  </si>
+  <si>
+    <t>Ilkal</t>
+  </si>
+  <si>
+    <t>ilkal</t>
+  </si>
+  <si>
+    <t>Handbag</t>
+  </si>
+  <si>
+    <t>handbag</t>
+  </si>
+  <si>
+    <t>Slingbag</t>
+  </si>
+  <si>
+    <t>slingbag</t>
+  </si>
+  <si>
+    <t>Handpurse</t>
+  </si>
+  <si>
+    <t>handpurse</t>
+  </si>
+  <si>
+    <t>Ladies Pouch</t>
+  </si>
+  <si>
+    <t>ladies-pouch</t>
+  </si>
+  <si>
+    <t>Beauty Products</t>
+  </si>
+  <si>
+    <t>beauty-products</t>
+  </si>
+  <si>
+    <t>Herbal Soap</t>
+  </si>
+  <si>
+    <t>herbal-soap</t>
+  </si>
+  <si>
+    <t>Sanitary Pads</t>
+  </si>
+  <si>
+    <t>sanitary-pads</t>
+  </si>
+  <si>
+    <t>Kids</t>
+  </si>
+  <si>
+    <t>kids</t>
+  </si>
+  <si>
+    <t>Baby Beds</t>
+  </si>
+  <si>
+    <t>baby-beds</t>
+  </si>
+  <si>
+    <t>Unisex</t>
+  </si>
+  <si>
+    <t>unisex</t>
+  </si>
+  <si>
+    <t>Mysore Peta</t>
+  </si>
+  <si>
+    <t>mysore-peta</t>
+  </si>
+  <si>
+    <t>Shawls</t>
+  </si>
+  <si>
+    <t>shawls</t>
+  </si>
+  <si>
+    <t>Lambani Bags</t>
+  </si>
+  <si>
+    <t>lambani-bags</t>
+  </si>
+  <si>
+    <t>Lambani Apparels</t>
+  </si>
+  <si>
+    <t>lambani-apparels</t>
+  </si>
+  <si>
+    <t>Lambani Dress</t>
+  </si>
+  <si>
+    <t>lambani-dress</t>
+  </si>
+  <si>
+    <t>Lambani Purse</t>
+  </si>
+  <si>
+    <t>lambani-purse</t>
+  </si>
+  <si>
+    <t>Pickles</t>
+  </si>
+  <si>
+    <t>pickles</t>
+  </si>
+  <si>
+    <t>Condiments</t>
+  </si>
+  <si>
+    <t>condiments</t>
+  </si>
+  <si>
+    <t>Beverages</t>
+  </si>
+  <si>
+    <t>beverages</t>
+  </si>
+  <si>
+    <t>Non-Alcoholic Drinks</t>
+  </si>
+  <si>
+    <t>non-alcoholic-drinks</t>
+  </si>
+  <si>
+    <t>Essential</t>
+  </si>
+  <si>
+    <t>essential</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>oil</t>
+  </si>
+  <si>
+    <t>Ghee</t>
+  </si>
+  <si>
+    <t>ghee</t>
+  </si>
+  <si>
+    <t>Papad</t>
+  </si>
+  <si>
+    <t>papad</t>
+  </si>
+  <si>
+    <t>Processed &amp; Packed foods</t>
+  </si>
+  <si>
+    <t>processed-&amp;-packed-foods</t>
+  </si>
+  <si>
+    <t>Spices</t>
+  </si>
+  <si>
+    <t>spices</t>
+  </si>
+  <si>
+    <t>Roti and Chutney</t>
+  </si>
+  <si>
+    <t>roti-and-chutney</t>
+  </si>
+  <si>
+    <t>Sweets</t>
+  </si>
+  <si>
+    <t>sweets</t>
+  </si>
+  <si>
+    <t>Tea &amp; Coffee</t>
+  </si>
+  <si>
+    <t>tea-&amp;-coffee</t>
+  </si>
+  <si>
+    <t>Apparels</t>
+  </si>
+  <si>
+    <t>apparels</t>
   </si>
 </sst>
 </file>
@@ -240,15 +582,19 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,7 +894,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -584,7 +930,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -595,13 +941,16 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="G2">
+        <v>0.0</v>
+      </c>
       <c r="H2">
-        <v>5</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -609,11 +958,17 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>0.0</v>
       </c>
       <c r="H3">
-        <v>5</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -626,11 +981,17 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0.0</v>
       </c>
       <c r="H4">
-        <v>5</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -643,14 +1004,17 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>0.0</v>
       </c>
       <c r="H5">
-        <v>6</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -664,13 +1028,16 @@
         <v>17</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
+      <c r="G6">
+        <v>0.0</v>
+      </c>
       <c r="H6">
-        <v>2</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -683,11 +1050,17 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>0.0</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -701,16 +1074,16 @@
         <v>21</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
-      <c r="F8">
-        <v>2</v>
+      <c r="G8">
+        <v>0.0</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -724,13 +1097,16 @@
         <v>23</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
+      <c r="G9">
+        <v>0.0</v>
+      </c>
       <c r="H9">
-        <v>5</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -746,8 +1122,11 @@
       <c r="E10">
         <v>1</v>
       </c>
+      <c r="G10">
+        <v>0.0</v>
+      </c>
       <c r="H10">
-        <v>5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -766,11 +1145,11 @@
       <c r="E11">
         <v>2</v>
       </c>
-      <c r="F11">
-        <v>2</v>
+      <c r="G11">
+        <v>0.0</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -783,11 +1162,17 @@
       <c r="C12" t="s">
         <v>29</v>
       </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
       <c r="E12">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>0.0</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -801,13 +1186,16 @@
         <v>31</v>
       </c>
       <c r="D13">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E13">
         <v>2</v>
       </c>
+      <c r="G13">
+        <v>0.0</v>
+      </c>
       <c r="H13">
-        <v>3</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -820,11 +1208,17 @@
       <c r="C14" t="s">
         <v>33</v>
       </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
       <c r="E14">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>0.0</v>
       </c>
       <c r="H14">
-        <v>5</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -838,16 +1232,16 @@
         <v>35</v>
       </c>
       <c r="D15">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
-      <c r="F15">
-        <v>1</v>
+      <c r="G15">
+        <v>0.0</v>
       </c>
       <c r="H15">
-        <v>5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -863,6 +1257,12 @@
       <c r="E16">
         <v>1</v>
       </c>
+      <c r="G16">
+        <v>0.0</v>
+      </c>
+      <c r="H16">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
@@ -875,10 +1275,16 @@
         <v>39</v>
       </c>
       <c r="D17">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E17">
         <v>2</v>
+      </c>
+      <c r="G17">
+        <v>0.0</v>
+      </c>
+      <c r="H17">
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -892,10 +1298,16 @@
         <v>41</v>
       </c>
       <c r="D18">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E18">
         <v>2</v>
+      </c>
+      <c r="G18">
+        <v>0.0</v>
+      </c>
+      <c r="H18">
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -911,8 +1323,11 @@
       <c r="E19">
         <v>1</v>
       </c>
+      <c r="G19">
+        <v>0.0</v>
+      </c>
       <c r="H19">
-        <v>1</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -926,10 +1341,16 @@
         <v>45</v>
       </c>
       <c r="D20">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E20">
         <v>2</v>
+      </c>
+      <c r="G20">
+        <v>0.0</v>
+      </c>
+      <c r="H20">
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -942,8 +1363,17 @@
       <c r="C21" t="s">
         <v>47</v>
       </c>
+      <c r="D21">
+        <v>18</v>
+      </c>
       <c r="E21">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>0.0</v>
+      </c>
+      <c r="H21">
+        <v>5.0</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -957,13 +1387,16 @@
         <v>49</v>
       </c>
       <c r="D22">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>0.0</v>
       </c>
       <c r="H22">
-        <v>3</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -976,16 +1409,22 @@
       <c r="C23" t="s">
         <v>51</v>
       </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
       <c r="E23">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>0.0</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>52</v>
@@ -997,12 +1436,18 @@
         <v>1</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>0.0</v>
+      </c>
+      <c r="H24">
+        <v>0.0</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>54</v>
@@ -1010,13 +1455,22 @@
       <c r="C25" t="s">
         <v>55</v>
       </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
       <c r="E25">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>0.0</v>
+      </c>
+      <c r="H25">
+        <v>0.0</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>56</v>
@@ -1025,15 +1479,21 @@
         <v>57</v>
       </c>
       <c r="D26">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>0.0</v>
+      </c>
+      <c r="H26">
+        <v>0.0</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>58</v>
@@ -1041,13 +1501,22 @@
       <c r="C27" t="s">
         <v>59</v>
       </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
       <c r="E27">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>0.0</v>
+      </c>
+      <c r="H27">
+        <v>0.0</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>60</v>
@@ -1055,13 +1524,22 @@
       <c r="C28" t="s">
         <v>61</v>
       </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
       <c r="E28">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>0.0</v>
+      </c>
+      <c r="H28">
+        <v>0.0</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>62</v>
@@ -1070,15 +1548,21 @@
         <v>63</v>
       </c>
       <c r="D29">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>0.0</v>
+      </c>
+      <c r="H29">
+        <v>0.0</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>64</v>
@@ -1086,12 +1570,1307 @@
       <c r="C30" t="s">
         <v>65</v>
       </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
       <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <v>0.0</v>
+      </c>
+      <c r="H30">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <v>0.0</v>
+      </c>
+      <c r="H31">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>0.0</v>
+      </c>
+      <c r="H32">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33">
+        <v>7</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="G33">
+        <v>0.0</v>
+      </c>
+      <c r="H33">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34">
+        <v>7</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="G34">
+        <v>0.0</v>
+      </c>
+      <c r="H34">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35">
+        <v>7</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="G35">
+        <v>0.0</v>
+      </c>
+      <c r="H35">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <v>0.0</v>
+      </c>
+      <c r="H36">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <v>0.0</v>
+      </c>
+      <c r="H37">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="G38">
+        <v>0.0</v>
+      </c>
+      <c r="H38">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="G39">
+        <v>0.0</v>
+      </c>
+      <c r="H39">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>0.0</v>
+      </c>
+      <c r="H40">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="G41">
+        <v>0.0</v>
+      </c>
+      <c r="H41">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="G42">
+        <v>0.0</v>
+      </c>
+      <c r="H42">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="G43">
+        <v>0.0</v>
+      </c>
+      <c r="H43">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44">
+        <v>8</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="G44">
+        <v>0.0</v>
+      </c>
+      <c r="H44">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="G45">
+        <v>0.0</v>
+      </c>
+      <c r="H45">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="G46">
+        <v>0.0</v>
+      </c>
+      <c r="H46">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="G47">
+        <v>0.0</v>
+      </c>
+      <c r="H47">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48">
+        <v>6</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+      <c r="G48">
+        <v>0.0</v>
+      </c>
+      <c r="H48">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49">
+        <v>10</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="G49">
+        <v>0.0</v>
+      </c>
+      <c r="H49">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50">
+        <v>10</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="G50">
+        <v>0.0</v>
+      </c>
+      <c r="H50">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51">
+        <v>10</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <v>0.0</v>
+      </c>
+      <c r="H51">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52">
+        <v>10</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+      <c r="G52">
+        <v>0.0</v>
+      </c>
+      <c r="H52">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" t="s">
+        <v>111</v>
+      </c>
+      <c r="D53">
+        <v>11</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="G53">
+        <v>0.0</v>
+      </c>
+      <c r="H53">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54">
+        <v>12</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="G54">
+        <v>0.0</v>
+      </c>
+      <c r="H54">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" t="s">
+        <v>115</v>
+      </c>
+      <c r="D55">
+        <v>12</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <v>0.0</v>
+      </c>
+      <c r="H55">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>116</v>
+      </c>
+      <c r="C56" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56">
+        <v>12</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="G56">
+        <v>0.0</v>
+      </c>
+      <c r="H56">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57">
+        <v>12</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <v>0.0</v>
+      </c>
+      <c r="H57">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" t="s">
+        <v>121</v>
+      </c>
+      <c r="D58">
+        <v>13</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="G58">
+        <v>0.0</v>
+      </c>
+      <c r="H58">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59">
+        <v>13</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+      <c r="G59">
+        <v>0.0</v>
+      </c>
+      <c r="H59">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>124</v>
+      </c>
+      <c r="C60" t="s">
+        <v>125</v>
+      </c>
+      <c r="D60">
+        <v>13</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+      <c r="G60">
+        <v>0.0</v>
+      </c>
+      <c r="H60">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" t="s">
+        <v>127</v>
+      </c>
+      <c r="D61">
+        <v>13</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+      <c r="G61">
+        <v>0.0</v>
+      </c>
+      <c r="H61">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62">
+        <v>14</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="G62">
+        <v>0.0</v>
+      </c>
+      <c r="H62">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>130</v>
+      </c>
+      <c r="C63" t="s">
+        <v>131</v>
+      </c>
+      <c r="D63">
+        <v>14</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="G63">
+        <v>0.0</v>
+      </c>
+      <c r="H63">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" t="s">
+        <v>133</v>
+      </c>
+      <c r="D64">
+        <v>14</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="G64">
+        <v>0.0</v>
+      </c>
+      <c r="H64">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>134</v>
+      </c>
+      <c r="C65" t="s">
+        <v>135</v>
+      </c>
+      <c r="E65">
         <v>1</v>
       </c>
+      <c r="G65">
+        <v>0.0</v>
+      </c>
+      <c r="H65">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>136</v>
+      </c>
+      <c r="C66" t="s">
+        <v>137</v>
+      </c>
+      <c r="D66">
+        <v>65</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="G66">
+        <v>0.0</v>
+      </c>
+      <c r="H66">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" t="s">
+        <v>139</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>0.0</v>
+      </c>
+      <c r="H67">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>140</v>
+      </c>
+      <c r="C68" t="s">
+        <v>141</v>
+      </c>
+      <c r="D68">
+        <v>67</v>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="G68">
+        <v>0.0</v>
+      </c>
+      <c r="H68">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="B69" t="s">
+        <v>142</v>
+      </c>
+      <c r="C69" t="s">
+        <v>143</v>
+      </c>
+      <c r="D69">
+        <v>67</v>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+      <c r="G69">
+        <v>0.0</v>
+      </c>
+      <c r="H69">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70">
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
+        <v>144</v>
+      </c>
+      <c r="C70" t="s">
+        <v>145</v>
+      </c>
+      <c r="D70">
+        <v>67</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="G70">
+        <v>0.0</v>
+      </c>
+      <c r="H70">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71">
+        <v>72</v>
+      </c>
+      <c r="B71" t="s">
+        <v>146</v>
+      </c>
+      <c r="C71" t="s">
+        <v>147</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>0.0</v>
+      </c>
+      <c r="H71">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>148</v>
+      </c>
+      <c r="C72" t="s">
+        <v>149</v>
+      </c>
+      <c r="D72">
+        <v>72</v>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+      <c r="G72">
+        <v>0.0</v>
+      </c>
+      <c r="H72">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73">
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
+        <v>150</v>
+      </c>
+      <c r="C73" t="s">
+        <v>151</v>
+      </c>
+      <c r="D73">
+        <v>72</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+      <c r="G73">
+        <v>0.0</v>
+      </c>
+      <c r="H73">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74">
+        <v>75</v>
+      </c>
+      <c r="B74" t="s">
+        <v>152</v>
+      </c>
+      <c r="C74" t="s">
+        <v>153</v>
+      </c>
+      <c r="D74">
+        <v>74</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+      <c r="G74">
+        <v>0.0</v>
+      </c>
+      <c r="H74">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>154</v>
+      </c>
+      <c r="C75" t="s">
+        <v>155</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>0.0</v>
+      </c>
+      <c r="H75">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>156</v>
+      </c>
+      <c r="C76" t="s">
+        <v>157</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="G76">
+        <v>0.0</v>
+      </c>
+      <c r="H76">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77">
+        <v>77</v>
+      </c>
+      <c r="B77" t="s">
+        <v>158</v>
+      </c>
+      <c r="C77" t="s">
+        <v>159</v>
+      </c>
+      <c r="D77">
+        <v>76</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="G77">
+        <v>0.0</v>
+      </c>
+      <c r="H77">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>160</v>
+      </c>
+      <c r="C78" t="s">
+        <v>161</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="G78">
+        <v>0.0</v>
+      </c>
+      <c r="H78">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>162</v>
+      </c>
+      <c r="C79" t="s">
+        <v>163</v>
+      </c>
+      <c r="D79">
+        <v>78</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+      <c r="G79">
+        <v>0.0</v>
+      </c>
+      <c r="H79">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>164</v>
+      </c>
+      <c r="C80" t="s">
+        <v>165</v>
+      </c>
+      <c r="D80">
+        <v>78</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="G80">
+        <v>0.0</v>
+      </c>
+      <c r="H80">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>166</v>
+      </c>
+      <c r="C81" t="s">
+        <v>167</v>
+      </c>
+      <c r="D81">
+        <v>78</v>
+      </c>
+      <c r="E81">
+        <v>2</v>
+      </c>
+      <c r="G81">
+        <v>0.0</v>
+      </c>
+      <c r="H81">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>168</v>
+      </c>
+      <c r="C82" t="s">
+        <v>169</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>0.0</v>
+      </c>
+      <c r="H82">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83">
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
+        <v>170</v>
+      </c>
+      <c r="C83" t="s">
+        <v>171</v>
+      </c>
+      <c r="D83">
+        <v>82</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="G83">
+        <v>0.0</v>
+      </c>
+      <c r="H83">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>172</v>
+      </c>
+      <c r="C84" t="s">
+        <v>173</v>
+      </c>
+      <c r="D84">
+        <v>82</v>
+      </c>
+      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="G84">
+        <v>0.0</v>
+      </c>
+      <c r="H84">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>174</v>
+      </c>
+      <c r="C85" t="s">
+        <v>175</v>
+      </c>
+      <c r="D85">
+        <v>82</v>
+      </c>
+      <c r="E85">
+        <v>2</v>
+      </c>
+      <c r="G85">
+        <v>0.0</v>
+      </c>
+      <c r="H85">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" t="s">
+        <v>177</v>
+      </c>
+      <c r="D86">
+        <v>82</v>
+      </c>
+      <c r="E86">
+        <v>2</v>
+      </c>
+      <c r="G86">
+        <v>0.0</v>
+      </c>
+      <c r="H86">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87">
+        <v>64</v>
+      </c>
+      <c r="B87" t="s">
+        <v>178</v>
+      </c>
+      <c r="C87" t="s">
+        <v>179</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="G87">
+        <v>0.0</v>
+      </c>
+      <c r="H87">
+        <v>0.0</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
@@ -1103,5 +2882,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>